<commit_message>
Reorganize, add DESE 2007 Database items
</commit_message>
<xml_diff>
--- a/test_data/codec/SensorData.xlsx
+++ b/test_data/codec/SensorData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\dev\scm\projects\dev_tools\python_tools\PTK\integration\IRAD_Runs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PaulLeopard\dev\py_base\DETk\database\test_data\codec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78A881F-2AF3-4124-B24D-CF72BB6281BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CB1EB6-7C97-4B50-94E1-AED258500D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="763" yWindow="985" windowWidth="23631" windowHeight="12283" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,12 +420,12 @@
   <dimension ref="A1:E315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.8" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -442,7 +442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -459,7 +459,7 @@
         <v>12.29041176470588</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>0.1669792993630573</v>
       </c>
@@ -476,7 +476,7 @@
         <v>12.37342574257425</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0.33395859872611472</v>
       </c>
@@ -493,7 +493,7 @@
         <v>12.280069306930701</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0.500937898089172</v>
       </c>
@@ -510,7 +510,7 @@
         <v>12.302029702970289</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>0.66791719745222933</v>
       </c>
@@ -527,7 +527,7 @@
         <v>12.27724752475247</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>0.83489649681528655</v>
       </c>
@@ -544,7 +544,7 @@
         <v>12.17378217821782</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1.001875796178344</v>
       </c>
@@ -561,7 +561,7 @@
         <v>12.15824752475247</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1.168855095541401</v>
       </c>
@@ -578,7 +578,7 @@
         <v>12.40913861386138</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1.335834394904458</v>
       </c>
@@ -595,7 +595,7 @@
         <v>12.433910891089109</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>1.5028136942675161</v>
       </c>
@@ -612,7 +612,7 @@
         <v>12.497049504950491</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1.6697929936305731</v>
       </c>
@@ -629,7 +629,7 @@
         <v>12.557534653465339</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>1.8367722929936301</v>
       </c>
@@ -646,7 +646,7 @@
         <v>12.30569306930693</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2.003751592356688</v>
       </c>
@@ -663,7 +663,7 @@
         <v>12.30475247524752</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2.170730891719745</v>
       </c>
@@ -680,7 +680,7 @@
         <v>12.32120792079207</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>2.337710191082802</v>
       </c>
@@ -697,7 +697,7 @@
         <v>12.2589207920792</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2.5046894904458599</v>
       </c>
@@ -714,7 +714,7 @@
         <v>12.41650495049505</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>2.6716687898089169</v>
       </c>
@@ -731,7 +731,7 @@
         <v>12.477821782178211</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>2.8386480891719752</v>
       </c>
@@ -748,7 +748,7 @@
         <v>12.52270297029702</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>3.0056273885350322</v>
       </c>
@@ -765,7 +765,7 @@
         <v>12.40277227722771</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>3.1726066878980901</v>
       </c>
@@ -782,7 +782,7 @@
         <v>12.568514851485141</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>3.3395859872611471</v>
       </c>
@@ -799,7 +799,7 @@
         <v>12.50167326732673</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>3.506565286624205</v>
       </c>
@@ -816,7 +816,7 @@
         <v>12.225059405940589</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>3.673544585987262</v>
       </c>
@@ -833,7 +833,7 @@
         <v>12.283722772277221</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>3.8405238853503199</v>
       </c>
@@ -850,7 +850,7 @@
         <v>12.33316831683168</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>4.0075031847133769</v>
       </c>
@@ -867,7 +867,7 @@
         <v>12.303841584158411</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>4.1744824840764343</v>
       </c>
@@ -884,7 +884,7 @@
         <v>12.40642574257425</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>4.3414617834394926</v>
       </c>
@@ -901,7 +901,7 @@
         <v>12.45678217821782</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>4.5084410828025492</v>
       </c>
@@ -918,7 +918,7 @@
         <v>12.454999999999989</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>4.6754203821656066</v>
       </c>
@@ -935,7 +935,7 @@
         <v>12.47599009900989</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>4.8423996815286632</v>
       </c>
@@ -952,7 +952,7 @@
         <v>12.37071287128712</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>5.0093789808917206</v>
       </c>
@@ -969,7 +969,7 @@
         <v>12.533722772277221</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>5.1763582802547772</v>
       </c>
@@ -986,7 +986,7 @@
         <v>12.46046534653464</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>5.3433375796178346</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>12.46321782178217</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>5.5103168789808912</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>12.44854455445544</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>5.6772961783439486</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>86.262089108910857</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>5.8442754777070052</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>86.008732673267275</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>6.0112547770700626</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>85.699138613861379</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>6.1782340764331192</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>85.436366336633725</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>6.3452133757961766</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>85.682712871287166</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>6.5121926751592332</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>85.442792079207948</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>6.6791719745222906</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>85.331980198019821</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>6.8461512738853481</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>85.156128712871265</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>7.0131305732484046</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>85.072752475247526</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>7.1801098726114621</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>85.163475247524744</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>7.3470891719745186</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>85.127732673267346</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>7.514068471337576</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>85.019594059405932</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>7.6810477707006326</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>84.98759405940595</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>7.84802707006369</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>84.925386138613874</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>8.0150063694267466</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>84.834841584158454</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>8.1819856687898032</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>84.814752475247545</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>8.3489649681528615</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>84.734277227722814</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>8.515944267515918</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>84.636435643564411</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>8.6829235668789746</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>84.537504950495034</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>8.8499028662420312</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>84.455029702970279</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>9.0168821656050895</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>84.526534653465319</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>9.183861464968146</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>84.405603960395993</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>9.3508407643312026</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>84.280188118811893</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>9.5178200636942609</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>84.281970297029659</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>9.6847993630573175</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>84.341504950495093</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>9.851778662420374</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>84.196801980198046</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>10.018757961783431</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>84.277415841584201</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>10.185737261146491</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>84.259970297029639</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>10.352716560509551</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>84.321346534653472</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>10.5196958598726</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>84.194089108910859</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>10.68667515923566</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>84.264584158415843</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>10.85365445859872</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>84.238950495049494</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>11.02063375796177</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>84.027356435643483</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>11.18761305732483</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>84.025544554455394</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>11.35459235668789</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>84.154722772277196</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>11.52157165605094</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>94.367366336633637</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>11.688550955414</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>95.560475247524707</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>11.85553025477706</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>93.713019801980224</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>12.02250955414012</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>96.008069306930722</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>12.189488853503169</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>95.868851485148582</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>12.356468152866229</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>95.651831683168311</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>12.52344745222929</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>95.493495049504887</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>12.690426751592341</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>95.277782178217805</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>12.857406050955399</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>95.209019801980219</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>13.024385350318459</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>94.981900990099021</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>13.19136464968151</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>98.248564356435651</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>13.358343949044571</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>98.401376237623822</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>13.525323248407631</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>100.4200396039604</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>13.692302547770691</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>99.822465346534699</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>13.85928184713374</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>99.838920792079293</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>14.0262611464968</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>100.0391584158417</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>14.19324044585986</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>99.63565346534655</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>14.36021974522291</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>99.348079207920804</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>14.52719904458597</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>99.335287128712807</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>14.69417834394903</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>99.284871287128681</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>14.86115764331208</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>99.477178217821731</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>15.02813694267514</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>99.40763366336634</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>15.1951162420382</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>99.265653465346531</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>15.36209554140126</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>99.22537623762372</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>15.529074840764309</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>99.350821782178187</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>15.696054140127369</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>99.233584158415823</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>15.86303343949043</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>99.154841584158405</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>16.030012738853479</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>98.88926732673265</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>16.196992038216539</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>98.714326732673229</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>16.363971337579599</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>99.03756435643561</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>16.530950636942659</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>98.75370297029697</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>16.697929936305709</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>98.704227722772259</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>16.864909235668769</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>98.561405940594142</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>17.031888535031829</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>98.666722772277211</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>17.198867834394889</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>98.718940594059376</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>17.365847133757939</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>98.696049504950452</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>17.532826433120999</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>98.559574257425766</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>17.699805732484059</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>98.400465346534673</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>17.866785031847112</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>98.286089108910929</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>18.033764331210168</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>98.467168316831717</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>18.200743630573228</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>98.3894752475248</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>18.367722929936281</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>98.498237623762449</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>18.534702229299342</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>98.382118811881227</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>18.701681528662402</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>98.336455445544601</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>18.868660828025451</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>98.289792079207899</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>19.035640127388511</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>98.199237623762357</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>19.202619426751571</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>88.028277227722754</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>19.369598726114631</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>106.31794059405939</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>19.536578025477681</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>67.50820792079206</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>19.703557324840741</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>70.690871287128687</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>19.870536624203801</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>70.298861386138583</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>20.037515923566851</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>70.294267326732665</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>20.204495222929911</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>70.025881188118831</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>20.371474522292971</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>70.025881188118817</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>20.538453821656031</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>69.84</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>20.70543312101908</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>69.760267326732617</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>20.87241242038214</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>69.972762376237625</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>21.039391719745201</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>69.637603960396021</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>21.20637101910825</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>69.784108910891021</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>21.37335031847131</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>69.459247524752527</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>21.54032961783437</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>69.495831683168376</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>21.70730891719743</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>69.665999999999968</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>21.87428821656048</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>69.474801980198023</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>22.04126751592354</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>69.615653465346526</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>22.2082468152866</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>69.513237623762393</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>22.375226114649649</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>69.376970297029757</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>22.542205414012709</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>69.470217821782256</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>22.70918471337577</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>69.18564356435644</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>22.876164012738819</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>69.320237623762409</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>23.043143312101879</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>69.242485148514902</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>23.210122611464939</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>69.379683168316888</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>23.377101910827999</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>69.099613861386189</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>23.544081210191049</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>69.032752475247491</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>23.711060509554109</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>69.017168316831658</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>23.878039808917169</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>68.92464356435643</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>24.045019108280218</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>87.778336633663358</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>24.211998407643279</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>83.101910891089162</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>24.378977707006339</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>82.616544554455473</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>24.545957006369399</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>82.403188118811912</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>24.712936305732448</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>82.200762376237549</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>24.879915605095508</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>82.049683168316747</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>25.046894904458561</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>82.01118811881183</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>25.213874203821621</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>81.991970297029653</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>25.380853503184682</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>81.600366336633655</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>25.547832802547742</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>81.982831683168243</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>25.714812101910791</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>81.651643564356419</v>
       </c>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>25.881791401273851</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>81.264366336633643</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>26.048770700636911</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>81.275356435643531</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>26.215749999999961</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>81.293673267326696</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>26.382729299363021</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>81.396247524752468</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>26.549708598726081</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>81.31383168316826</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>26.716687898089141</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>81.223108910891071</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>26.883667197452191</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>81.099544554455434</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>27.050646496815251</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>81.148970297029706</v>
       </c>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>27.217625796178311</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>81.27621782178214</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
         <v>27.38460509554136</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>81.164524752475245</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>27.55158439490442</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>81.064732673267329</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>27.71856369426748</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>80.919079207920774</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>27.88554299363053</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>80.869603960396063</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>28.05252229299359</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>80.85863366336639</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>28.21950159235665</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>81.023475247524729</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>28.38648089171971</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>80.850405940594072</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>28.55346019108276</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>80.94379207920791</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>28.72043949044582</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>80.858653465346549</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>28.88741878980888</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>80.524356435643568</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
         <v>29.054398089171929</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>80.474009900990055</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>29.221377388534989</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>80.319198019801959</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
         <v>29.38835668789805</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>80.414455445544533</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>29.55533598726111</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>80.332990099009848</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>29.722315286624159</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>80.096009900990083</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>29.889294585987219</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>80.073148514851482</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
         <v>30.056273885350279</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>79.931386138613874</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>30.223253184713329</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>80.032910891089131</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
         <v>30.390232484076389</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>79.717079207920833</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
         <v>30.557211783439449</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>79.685059405940606</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
         <v>30.724191082802509</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>79.813247524752512</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
         <v>30.891170382165559</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>79.776594059405951</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
         <v>31.058149681528619</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>79.616326732673244</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
         <v>31.225128980891679</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>79.531168316831682</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="3">
         <v>31.392108280254732</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>79.318702970297011</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
         <v>31.559087579617788</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>79.637455445544589</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="3">
         <v>31.726066878980848</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>79.160217821782183</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
         <v>31.893046178343901</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>79.435910891089051</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="3">
         <v>32.060025477706958</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>79.521108910891058</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
         <v>32.227004777070007</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>79.261930693069317</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
         <v>32.393984076433078</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>79.315930693069291</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
         <v>32.560963375796128</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>79.402049504950426</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="3">
         <v>32.727942675159191</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>79.304039603960362</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="3">
         <v>32.894921974522248</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>79.26834653465346</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="3">
         <v>33.061901273885297</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>79.067742574257437</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="3">
         <v>33.228880573248361</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>78.915782178217881</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="3">
         <v>33.395859872611418</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>78.891960396039664</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="3">
         <v>33.562839171974467</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>78.967940594059428</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="3">
         <v>33.729818471337531</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>78.729108910891142</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="3">
         <v>33.896797770700587</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>78.76847524752479</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="3">
         <v>34.063777070063637</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>78.727306930693103</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="3">
         <v>34.2307563694267</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>78.691544554455518</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="3">
         <v>34.397735668789757</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>78.623980198019851</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="3">
         <v>34.564714968152821</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>78.623980198019879</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="3">
         <v>34.731694267515877</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>78.555346534653509</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="3">
         <v>34.898673566878948</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>78.767504950495109</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="3">
         <v>35.065652866241997</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>78.815980198019844</v>
       </c>
     </row>
-    <row r="213" spans="1:5">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="3">
         <v>35.232632165605068</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>78.750168316831733</v>
       </c>
     </row>
-    <row r="214" spans="1:5">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="3">
         <v>35.399611464968118</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>78.718148514851521</v>
       </c>
     </row>
-    <row r="215" spans="1:5">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="3">
         <v>35.566590764331188</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>78.660584158415872</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="3">
         <v>35.733570063694252</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>78.7346039603961</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="3">
         <v>35.900549363057308</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>78.677009900990129</v>
       </c>
     </row>
-    <row r="218" spans="1:5">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="3">
         <v>36.067528662420372</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>78.70351485148521</v>
       </c>
     </row>
-    <row r="219" spans="1:5">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="3">
         <v>36.234507961783429</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>78.539801980198035</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="3">
         <v>36.401487261146492</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>78.56358415841585</v>
       </c>
     </row>
-    <row r="221" spans="1:5">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="3">
         <v>36.568466560509563</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>78.26048514851486</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="3">
         <v>36.735445859872613</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>78.255960396039598</v>
       </c>
     </row>
-    <row r="223" spans="1:5">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="3">
         <v>36.902425159235683</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>78.215623762376268</v>
       </c>
     </row>
-    <row r="224" spans="1:5">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="3">
         <v>37.069404458598733</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>78.021465346534669</v>
       </c>
     </row>
-    <row r="225" spans="1:5">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="3">
         <v>37.236383757961796</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>77.994019801980215</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="3">
         <v>37.40336305732486</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>78.053504950495096</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="3">
         <v>37.570342356687917</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>77.972940594059438</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="3">
         <v>37.73732165605098</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>77.686247524752474</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="3">
         <v>37.904300955414037</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>77.840118811881226</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="3">
         <v>38.071280254777101</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>77.545227722772239</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="3">
         <v>38.238259554140157</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>77.428891089108902</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="3">
         <v>38.405238853503221</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>77.294277227722802</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" s="3">
         <v>38.572218152866277</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>77.088574257425776</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="3">
         <v>38.739197452229341</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>77.162594059405947</v>
       </c>
     </row>
-    <row r="235" spans="1:5">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" s="3">
         <v>38.906176751592398</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>77.012633663366387</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" s="3">
         <v>39.073156050955468</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>77.094900990099035</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" s="3">
         <v>39.240135350318518</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>77.460960396039638</v>
       </c>
     </row>
-    <row r="238" spans="1:5">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="3">
         <v>39.407114649681589</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>77.208287128712897</v>
       </c>
     </row>
-    <row r="239" spans="1:5">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="3">
         <v>39.574093949044652</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>76.981534653465346</v>
       </c>
     </row>
-    <row r="240" spans="1:5">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="3">
         <v>39.741073248407709</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>76.927475247524754</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" s="3">
         <v>39.908052547770772</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>76.847851485148482</v>
       </c>
     </row>
-    <row r="242" spans="1:5">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" s="3">
         <v>40.075031847133829</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>76.790168316831668</v>
       </c>
     </row>
-    <row r="243" spans="1:5">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" s="3">
         <v>40.242011146496893</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>76.538267326732665</v>
       </c>
     </row>
-    <row r="244" spans="1:5">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="3">
         <v>40.408990445859949</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>76.421990099009889</v>
       </c>
     </row>
-    <row r="245" spans="1:5">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="3">
         <v>40.575969745223013</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>76.52912871287127</v>
       </c>
     </row>
-    <row r="246" spans="1:5">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" s="3">
         <v>40.742949044586076</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>76.394514851485141</v>
       </c>
     </row>
-    <row r="247" spans="1:5">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="3">
         <v>40.909928343949133</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>76.466861386138604</v>
       </c>
     </row>
-    <row r="248" spans="1:5">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="3">
         <v>41.076907643312197</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>76.41828712871289</v>
       </c>
     </row>
-    <row r="249" spans="1:5">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="3">
         <v>41.243886942675253</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>76.604247524752495</v>
       </c>
     </row>
-    <row r="250" spans="1:5">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="3">
         <v>41.410866242038317</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>76.588683168316848</v>
       </c>
     </row>
-    <row r="251" spans="1:5">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="3">
         <v>41.577845541401381</v>
       </c>
@@ -4692,7 +4692,7 @@
         <v>76.213148514851582</v>
       </c>
     </row>
-    <row r="252" spans="1:5">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" s="3">
         <v>41.744824840764437</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>76.117980198019822</v>
       </c>
     </row>
-    <row r="253" spans="1:5">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="3">
         <v>41.911804140127501</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>76.193039603960443</v>
       </c>
     </row>
-    <row r="254" spans="1:5">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="3">
         <v>42.078783439490557</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>75.936534653465401</v>
       </c>
     </row>
-    <row r="255" spans="1:5">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="3">
         <v>42.245762738853621</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>76.000693069306976</v>
       </c>
     </row>
-    <row r="256" spans="1:5">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" s="3">
         <v>42.412742038216678</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>75.932900990099057</v>
       </c>
     </row>
-    <row r="257" spans="1:5">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" s="3">
         <v>42.579721337579741</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>76.02176237623766</v>
       </c>
     </row>
-    <row r="258" spans="1:5">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" s="3">
         <v>42.746700636942798</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>75.767158415841578</v>
       </c>
     </row>
-    <row r="259" spans="1:5">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" s="3">
         <v>42.913679936305861</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>75.779999999999987</v>
       </c>
     </row>
-    <row r="260" spans="1:5">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="3">
         <v>43.080659235668932</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>75.970455445544602</v>
       </c>
     </row>
-    <row r="261" spans="1:5">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" s="3">
         <v>43.247638535031989</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>75.587871287128678</v>
       </c>
     </row>
-    <row r="262" spans="1:5">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" s="3">
         <v>43.414617834395052</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>75.653722772277206</v>
       </c>
     </row>
-    <row r="263" spans="1:5">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" s="3">
         <v>43.581597133758109</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>75.587851485148505</v>
       </c>
     </row>
-    <row r="264" spans="1:5">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" s="3">
         <v>43.748576433121173</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>75.590584158415822</v>
       </c>
     </row>
-    <row r="265" spans="1:5">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" s="3">
         <v>43.915555732484229</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>75.629920792079204</v>
       </c>
     </row>
-    <row r="266" spans="1:5">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" s="3">
         <v>44.082535031847293</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>75.35549504950491</v>
       </c>
     </row>
-    <row r="267" spans="1:5">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" s="3">
         <v>44.249514331210349</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>75.404009900990076</v>
       </c>
     </row>
-    <row r="268" spans="1:5">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" s="3">
         <v>44.416493630573413</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>75.320702970296978</v>
       </c>
     </row>
-    <row r="269" spans="1:5">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" s="3">
         <v>44.58347292993647</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>75.055118811881201</v>
       </c>
     </row>
-    <row r="270" spans="1:5">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" s="3">
         <v>44.750452229299533</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>74.914079207920793</v>
       </c>
     </row>
-    <row r="271" spans="1:5">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" s="3">
         <v>44.917431528662597</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>74.961673267326745</v>
       </c>
     </row>
-    <row r="272" spans="1:5">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" s="3">
         <v>45.084410828025653</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>75.034029702970315</v>
       </c>
     </row>
-    <row r="273" spans="1:5">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" s="3">
         <v>45.251390127388717</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>74.996495049504972</v>
       </c>
     </row>
-    <row r="274" spans="1:5">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" s="3">
         <v>45.418369426751767</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>74.944306930693031</v>
       </c>
     </row>
-    <row r="275" spans="1:5">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" s="3">
         <v>45.585348726114837</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>74.846326732673276</v>
       </c>
     </row>
-    <row r="276" spans="1:5">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" s="3">
         <v>45.752328025477901</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>74.556019801980199</v>
       </c>
     </row>
-    <row r="277" spans="1:5">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" s="3">
         <v>45.919307324840958</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>74.566029702970354</v>
       </c>
     </row>
-    <row r="278" spans="1:5">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" s="3">
         <v>46.086286624204021</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>74.292297029702993</v>
       </c>
     </row>
-    <row r="279" spans="1:5">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" s="3">
         <v>46.253265923567078</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>74.174079207920826</v>
       </c>
     </row>
-    <row r="280" spans="1:5">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" s="3">
         <v>46.420245222930141</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>74.215267326732729</v>
       </c>
     </row>
-    <row r="281" spans="1:5">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" s="3">
         <v>46.587224522293212</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>74.005792079207936</v>
       </c>
     </row>
-    <row r="282" spans="1:5">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" s="3">
         <v>46.754203821656262</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>73.854891089108932</v>
       </c>
     </row>
-    <row r="283" spans="1:5">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" s="3">
         <v>46.921183121019332</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>73.718465346534643</v>
       </c>
     </row>
-    <row r="284" spans="1:5">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" s="3">
         <v>47.088162420382382</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>73.563712871287066</v>
       </c>
     </row>
-    <row r="285" spans="1:5">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" s="3">
         <v>47.255141719745453</v>
       </c>
@@ -5270,7 +5270,7 @@
         <v>73.239544554455478</v>
       </c>
     </row>
-    <row r="286" spans="1:5">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" s="3">
         <v>47.422121019108509</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>13.52695049504951</v>
       </c>
     </row>
-    <row r="287" spans="1:5">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" s="3">
         <v>47.589100318471573</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>13.019089108910901</v>
       </c>
     </row>
-    <row r="288" spans="1:5">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" s="3">
         <v>47.756079617834629</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>13.06022772277227</v>
       </c>
     </row>
-    <row r="289" spans="1:5">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" s="3">
         <v>47.923058917197693</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>73.119534653465408</v>
       </c>
     </row>
-    <row r="290" spans="1:5">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" s="3">
         <v>48.09003821656075</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>72.953762376237634</v>
       </c>
     </row>
-    <row r="291" spans="1:5">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" s="3">
         <v>48.257017515923813</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>72.790762376237637</v>
       </c>
     </row>
-    <row r="292" spans="1:5">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" s="3">
         <v>48.42399681528687</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>72.670920792079215</v>
       </c>
     </row>
-    <row r="293" spans="1:5">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" s="3">
         <v>48.590976114649933</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>72.651673267326757</v>
       </c>
     </row>
-    <row r="294" spans="1:5">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" s="3">
         <v>48.75795541401299</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>72.247257425742561</v>
       </c>
     </row>
-    <row r="295" spans="1:5">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" s="3">
         <v>48.924934713376047</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>72.23719801980198</v>
       </c>
     </row>
-    <row r="296" spans="1:5">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" s="3">
         <v>49.091914012739117</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>71.836970297029694</v>
       </c>
     </row>
-    <row r="297" spans="1:5">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" s="3">
         <v>49.258893312102167</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>71.564009900990087</v>
       </c>
     </row>
-    <row r="298" spans="1:5">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" s="3">
         <v>49.425872611465238</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>71.572267326732657</v>
       </c>
     </row>
-    <row r="299" spans="1:5">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" s="3">
         <v>49.592851910828287</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>71.208712871287133</v>
       </c>
     </row>
-    <row r="300" spans="1:5">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" s="3">
         <v>49.759831210191358</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>70.705475247524717</v>
       </c>
     </row>
-    <row r="301" spans="1:5">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" s="3">
         <v>49.926810509554421</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>70.443544554455414</v>
       </c>
     </row>
-    <row r="302" spans="1:5">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" s="3">
         <v>50.093789808917478</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>70.211762376237701</v>
       </c>
     </row>
-    <row r="303" spans="1:5">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" s="3">
         <v>50.260769108280542</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>69.902257425742548</v>
       </c>
     </row>
-    <row r="304" spans="1:5">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" s="3">
         <v>50.427748407643598</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>69.624782178217856</v>
       </c>
     </row>
-    <row r="305" spans="1:5">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" s="3">
         <v>50.594727707006662</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>69.385237623762393</v>
       </c>
     </row>
-    <row r="306" spans="1:5">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" s="3">
         <v>50.761707006369733</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>69.134425742574265</v>
       </c>
     </row>
-    <row r="307" spans="1:5">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" s="3">
         <v>50.928686305732782</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>68.734128712871282</v>
       </c>
     </row>
-    <row r="308" spans="1:5">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" s="3">
         <v>51.095665605095853</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>68.457564356435611</v>
       </c>
     </row>
-    <row r="309" spans="1:5">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" s="3">
         <v>51.262644904458902</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>68.104970297029723</v>
       </c>
     </row>
-    <row r="310" spans="1:5">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" s="3">
         <v>51.429624203821973</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>67.720811881188084</v>
       </c>
     </row>
-    <row r="311" spans="1:5">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" s="3">
         <v>51.59660350318503</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>67.32332673267328</v>
       </c>
     </row>
-    <row r="312" spans="1:5">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312" s="3">
         <v>51.763582802548093</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>66.922158415841551</v>
       </c>
     </row>
-    <row r="313" spans="1:5">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313" s="3">
         <v>51.93056210191115</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>66.262396039603942</v>
       </c>
     </row>
-    <row r="314" spans="1:5">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314" s="3">
         <v>52.097541401274214</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>13.32362376237624</v>
       </c>
     </row>
-    <row r="315" spans="1:5">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315" s="3">
         <v>52.26452070063727</v>
       </c>
@@ -5782,5 +5782,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 DESE Research, Inc.</oddFooter>
+  </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{3a1c331b-5232-43a0-827b-34eef4b3955f}" enabled="1" method="Privileged" siteId="{3701aadf-5391-43be-bb84-25a015a895f5}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>